<commit_message>
added my SSR doc
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VehansAyvazi\Desktop\MedVoice_Internship\medvoice\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="516" yWindow="612" windowWidth="15996" windowHeight="9204"/>
+    <workbookView xWindow="510" yWindow="615" windowWidth="15990" windowHeight="9210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -152,6 +157,18 @@
   </si>
   <si>
     <t>nitish072492@gmail.com</t>
+  </si>
+  <si>
+    <t>Vehans Ayvazi</t>
+  </si>
+  <si>
+    <t>(818) 383-0946</t>
+  </si>
+  <si>
+    <t>vehansayvazi5@gmail.com</t>
+  </si>
+  <si>
+    <t>Display Data</t>
   </si>
 </sst>
 </file>
@@ -196,10 +213,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -210,6 +228,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -258,7 +279,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -293,7 +314,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -502,20 +523,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,7 +550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -540,7 +561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -554,7 +575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -568,7 +589,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -582,7 +603,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -596,7 +617,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -610,7 +631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -624,7 +645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -638,7 +659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -652,7 +673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -666,7 +687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -680,7 +701,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -691,7 +712,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -700,11 +721,26 @@
       </c>
       <c r="C14" s="2" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C14" r:id="rId1"/>
+    <hyperlink ref="C15" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>